<commit_message>
the master keeps getting better
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\elemental\vindenatt.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450BC60F-88BA-4368-BABC-AC51F41087F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84D91DB-A3F8-4B23-A095-E51FE7030DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{785EF7B0-BCEA-4ABB-8F17-D9A2C5203060}"/>
   </bookViews>
@@ -575,7 +575,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -682,6 +682,7 @@
       <c r="C8">
         <v>6</v>
       </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
@@ -693,6 +694,7 @@
       <c r="C9">
         <v>7</v>
       </c>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -704,6 +706,7 @@
       <c r="C10">
         <v>8</v>
       </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
@@ -715,6 +718,7 @@
       <c r="C11">
         <v>9</v>
       </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
@@ -726,6 +730,7 @@
       <c r="C12">
         <v>10</v>
       </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" s="1"/>

</xml_diff>